<commit_message>
Made little changes to ERD, customer detail added 1. added customer detail to excel 2. made little changes to ERD, making full name derieved 3. The DDl and DML script was altered and now it works perfect and the whole database seems logical now
</commit_message>
<xml_diff>
--- a/ERD/Fintech-lab.xlsx
+++ b/ERD/Fintech-lab.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaiwant/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaiwant/repos/Jaiwant_230958058_fintech/ERD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FF57BA-1ABC-C046-B4C7-1C3387AA0BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F766C1C1-B002-9148-96ED-5806CBB958D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" activeTab="4" xr2:uid="{447D3D2B-46EE-6D43-A9A3-41EC29166205}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="CUST_NAME" sheetId="3" r:id="rId2"/>
     <sheet name="CUST_POI" sheetId="5" r:id="rId3"/>
     <sheet name="CUST_ADDRESS" sheetId="6" r:id="rId4"/>
-    <sheet name="CUST_NAME (2)" sheetId="7" r:id="rId5"/>
+    <sheet name="CUST_DETAILS" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="145">
   <si>
     <t>Customer Identification</t>
   </si>
@@ -393,13 +393,97 @@
   </si>
   <si>
     <t>address value for the component type chosen</t>
+  </si>
+  <si>
+    <t>Customer Details</t>
+  </si>
+  <si>
+    <t>CUST_DETAILS</t>
+  </si>
+  <si>
+    <t>Used to store the customer details, like name, contact, etc</t>
+  </si>
+  <si>
+    <t>Customer type</t>
+  </si>
+  <si>
+    <t>CSTDET_TYPE</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>Customer type, like Individual,etc</t>
+  </si>
+  <si>
+    <t>Customer Full Name</t>
+  </si>
+  <si>
+    <t>CSTDET_FULL_NAME</t>
+  </si>
+  <si>
+    <t>Full name of the customer, extracted from the CUST_NAME table</t>
+  </si>
+  <si>
+    <t>Customer DOB</t>
+  </si>
+  <si>
+    <t>CSTDET_DOB</t>
+  </si>
+  <si>
+    <t>Date of Birth of the customer</t>
+  </si>
+  <si>
+    <t>Customer status</t>
+  </si>
+  <si>
+    <t>CSTDET_STATUS</t>
+  </si>
+  <si>
+    <t>Status of the customer like active, dormant, etc</t>
+  </si>
+  <si>
+    <t>CSTDET_CONTACT</t>
+  </si>
+  <si>
+    <t>contact number of the customer</t>
+  </si>
+  <si>
+    <t>CSTDET_MOBILE</t>
+  </si>
+  <si>
+    <t>Customer mobile number</t>
+  </si>
+  <si>
+    <t>Customer contact number</t>
+  </si>
+  <si>
+    <t>mobile number of the customer</t>
+  </si>
+  <si>
+    <t>Customer email</t>
+  </si>
+  <si>
+    <t>CSTDET_EMAIL</t>
+  </si>
+  <si>
+    <t>Email ID of the customer</t>
+  </si>
+  <si>
+    <t>Customer Country of Origination</t>
+  </si>
+  <si>
+    <t>CSTDET_COUNTRY</t>
+  </si>
+  <si>
+    <t>Country of origin of the customer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,6 +507,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -459,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -482,33 +572,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -518,7 +582,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,12 +959,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -882,34 +973,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -926,24 +1017,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1044,116 +1135,444 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="14"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD60044C-D92D-2147-8FDD-EB0CD7E1722E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="13"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="14"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="21"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D5"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
@@ -1179,334 +1598,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD60044C-D92D-2147-8FDD-EB0CD7E1722E}">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="21"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-    </row>
-  </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3736C865-4DA7-FE44-B8BE-550178FFCCD7}">
   <dimension ref="A1:D23"/>
@@ -1524,12 +1615,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1538,34 +1629,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1582,27 +1673,27 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B9" t="s">
@@ -1805,15 +1896,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1836,12 +1927,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1850,34 +1941,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1894,27 +1985,27 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="10" t="s">
         <v>102</v>
       </c>
       <c r="B9" t="s">
@@ -2012,107 +2103,124 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="20" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="20" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="20" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="14"/>
+      <c r="A21" s="21"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C24:C25"/>
@@ -2125,23 +2233,6 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2149,10 +2240,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222693BF-2BFF-A046-AB6E-554C709C3F5D}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,12 +2255,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
+      <c r="A1" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2178,34 +2269,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="17"/>
+      <c r="A3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="14"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -2222,254 +2313,294 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
-        <v>55</v>
+      <c r="A9" s="23" t="s">
+        <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>125</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
+      <c r="A11" t="s">
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
+      </c>
+      <c r="C13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B18" t="s">
         <v>62</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B19" t="s">
         <v>63</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C19" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+    <row r="20" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B20" t="s">
         <v>64</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B21" t="s">
         <v>65</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="22" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B22" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C22" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D22" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B23" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C23" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D23" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="13" t="s">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B24" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C24" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D24" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="14"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="25" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B25" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C25" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="26" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B26" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C26" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D26" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
+  <mergeCells count="9">
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Saving as a checkpoint 1. going to be experimenting, if smtg goes wrong, Ill rollback
</commit_message>
<xml_diff>
--- a/ERD/Fintech-lab.xlsx
+++ b/ERD/Fintech-lab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaiwant/repos/Jaiwant_230958058_fintech/ERD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F766C1C1-B002-9148-96ED-5806CBB958D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A87F2F-2286-544B-8DE2-6AD31E71134B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16540" activeTab="4" xr2:uid="{447D3D2B-46EE-6D43-A9A3-41EC29166205}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="155">
   <si>
     <t>Customer Identification</t>
   </si>
@@ -383,9 +383,6 @@
     <t>CSTADD_ACPT_TS</t>
   </si>
   <si>
-    <t>CSTADd_ACPT_TS_UTC_OFST</t>
-  </si>
-  <si>
     <t>CSTADD_UUID</t>
   </si>
   <si>
@@ -477,6 +474,39 @@
   </si>
   <si>
     <t>Country of origin of the customer</t>
+  </si>
+  <si>
+    <t>CSTADD_ACPT_TS_UTC_OFST</t>
+  </si>
+  <si>
+    <t>CSTDET_EFCTV_DATE</t>
+  </si>
+  <si>
+    <t>CSTDET_CRUD_VALUE</t>
+  </si>
+  <si>
+    <t>CSTDET_USER_ID</t>
+  </si>
+  <si>
+    <t>CSTDET_WS_ID</t>
+  </si>
+  <si>
+    <t>CSTDET_PRGM_ID</t>
+  </si>
+  <si>
+    <t>CSTDET_HOST_TS</t>
+  </si>
+  <si>
+    <t>CSTDET_LOCAL_TS</t>
+  </si>
+  <si>
+    <t>CSTDET_ACPT_TS</t>
+  </si>
+  <si>
+    <t>CSTDET_ACPT_TS_UTC_OFST</t>
+  </si>
+  <si>
+    <t>CSTDET_UUID</t>
   </si>
 </sst>
 </file>
@@ -573,6 +603,31 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -585,31 +640,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,12 +989,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -973,34 +1003,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1017,24 +1047,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1135,444 +1165,116 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="20"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="20"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="15"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="A3:A5"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD60044C-D92D-2147-8FDD-EB0CD7E1722E}">
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>61</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="20"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-    </row>
-  </sheetData>
-  <mergeCells count="29">
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:D5"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
@@ -1598,6 +1300,334 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD60044C-D92D-2147-8FDD-EB0CD7E1722E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3736C865-4DA7-FE44-B8BE-550178FFCCD7}">
   <dimension ref="A1:D23"/>
@@ -1615,12 +1645,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1629,34 +1659,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1673,24 +1703,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
@@ -1915,7 +1945,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1927,12 +1957,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1941,34 +1971,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1985,24 +2015,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
@@ -2015,7 +2045,7 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2029,7 +2059,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2103,124 +2133,107 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="20"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="20"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="20"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="19" t="s">
+      <c r="A22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="19"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="19"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="C24:C25"/>
@@ -2233,6 +2246,23 @@
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2243,7 +2273,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2255,12 +2285,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="A1" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2269,34 +2299,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="C3" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -2313,135 +2343,135 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" t="s">
         <v>120</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>121</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>122</v>
-      </c>
-      <c r="D9" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
         <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>125</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" t="s">
         <v>127</v>
-      </c>
-      <c r="B11" t="s">
-        <v>128</v>
       </c>
       <c r="C11" t="s">
         <v>83</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" t="s">
         <v>130</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" t="s">
         <v>131</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" t="s">
         <v>133</v>
-      </c>
-      <c r="C13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
         <v>139</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" t="s">
         <v>140</v>
-      </c>
-      <c r="C15" t="s">
-        <v>122</v>
-      </c>
-      <c r="D15" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>141</v>
+      </c>
+      <c r="B16" t="s">
         <v>142</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" t="s">
         <v>143</v>
-      </c>
-      <c r="C16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D16" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2449,7 +2479,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -2463,7 +2493,7 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -2477,7 +2507,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -2491,7 +2521,7 @@
         <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>148</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -2505,7 +2535,7 @@
         <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -2519,7 +2549,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>66</v>
+        <v>150</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>19</v>
@@ -2533,7 +2563,7 @@
         <v>38</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>67</v>
+        <v>151</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>19</v>
@@ -2547,7 +2577,7 @@
         <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>152</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>19</v>
@@ -2561,7 +2591,7 @@
         <v>40</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>69</v>
+        <v>153</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>19</v>
@@ -2575,7 +2605,7 @@
         <v>41</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
commmiting just before branching
</commit_message>
<xml_diff>
--- a/ERD/Fintech-lab.xlsx
+++ b/ERD/Fintech-lab.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jaiwant/repos/Jaiwant_230958058_fintech/ERD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA1C9EB-52ED-1944-83C7-96E3F6440CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB542EA-FE36-4243-A3A8-033163C8C17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16540" activeTab="6" xr2:uid="{447D3D2B-46EE-6D43-A9A3-41EC29166205}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16540" activeTab="4" xr2:uid="{447D3D2B-46EE-6D43-A9A3-41EC29166205}"/>
   </bookViews>
   <sheets>
     <sheet name="CUST_ID" sheetId="1" r:id="rId1"/>
     <sheet name="CUST_NAME" sheetId="3" r:id="rId2"/>
     <sheet name="CUST_POI" sheetId="5" r:id="rId3"/>
-    <sheet name="CUST_ADDRESS" sheetId="6" r:id="rId4"/>
-    <sheet name="CUST_DETAILS" sheetId="7" r:id="rId5"/>
-    <sheet name="CUST_CL" sheetId="9" r:id="rId6"/>
-    <sheet name="CUST_SIGNIN" sheetId="11" r:id="rId7"/>
+    <sheet name="FIN_INSTITUTIONS" sheetId="12" r:id="rId4"/>
+    <sheet name="CUST_ADDRESS" sheetId="6" r:id="rId5"/>
+    <sheet name="CUST_DETAILS" sheetId="7" r:id="rId6"/>
+    <sheet name="CUST_CL" sheetId="9" r:id="rId7"/>
+    <sheet name="CUST_SIGNIN" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="227">
   <si>
     <t>Customer Identification</t>
   </si>
@@ -494,9 +495,6 @@
   </si>
   <si>
     <t>Full name of the customer, by merging all the first, middle and last names</t>
-  </si>
-  <si>
-    <t>I have a doubt, wiz when updated, I create a new row right? Or else  I update the same row and make the CRUD value as 'U', if so then it is pointless right</t>
   </si>
   <si>
     <t>Customer address identifier</t>
@@ -677,6 +675,63 @@
   </si>
   <si>
     <t>Customer password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INSTITUTION_ID </t>
+  </si>
+  <si>
+    <t>INSTITUTION_NAME</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Institution logical database ID</t>
+  </si>
+  <si>
+    <t>Institution name</t>
+  </si>
+  <si>
+    <t>INST_EFCTV_DATE</t>
+  </si>
+  <si>
+    <t>INST_CRUD_VALUE</t>
+  </si>
+  <si>
+    <t>INST_USER_ID</t>
+  </si>
+  <si>
+    <t>INST_WS_ID</t>
+  </si>
+  <si>
+    <t>INST_PRGM_ID</t>
+  </si>
+  <si>
+    <t>INST_HOST_TS</t>
+  </si>
+  <si>
+    <t>INST_LOCAL_TS</t>
+  </si>
+  <si>
+    <t>INST_ACPT_TS</t>
+  </si>
+  <si>
+    <t>INST_ACPT_TS_UTC_OFST</t>
+  </si>
+  <si>
+    <t>INST_UUID</t>
+  </si>
+  <si>
+    <t>FIN_INSTITUTIONS</t>
+  </si>
+  <si>
+    <t>Used to store the logical database ID of the financial institution, this is usefull if we have a multi-tenant database, we can identify each institutions record</t>
+  </si>
+  <si>
+    <t>Finincial institutions</t>
+  </si>
+  <si>
+    <t>ID assigned to the financial institution</t>
   </si>
 </sst>
 </file>
@@ -788,6 +843,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -803,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -825,14 +882,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1184,12 +1239,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1198,34 +1253,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1242,34 +1297,34 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
@@ -1280,7 +1335,7 @@
         <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" t="s">
         <v>28</v>
@@ -1360,117 +1415,117 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>153</v>
+      <c r="C26" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1526,12 +1581,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1540,34 +1595,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1584,24 +1639,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>154</v>
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
@@ -1611,7 +1666,7 @@
         <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
         <v>53</v>
@@ -1702,117 +1757,117 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>159</v>
-      </c>
-      <c r="B26" s="26" t="s">
+      <c r="A26" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="C26" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>153</v>
+      <c r="D26" s="13" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1868,12 +1923,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1882,34 +1937,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1926,24 +1981,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>154</v>
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
@@ -1953,7 +2008,7 @@
         <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
         <v>73</v>
@@ -2142,17 +2197,17 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>153</v>
+      <c r="C23" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2172,10 +2227,283 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{821BAE8B-C65C-7D42-9F96-01B3D4596880}">
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="D3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:D5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{889447E6-3B45-6845-AF80-CC1531D49E99}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -2188,12 +2516,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2202,34 +2530,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -2246,24 +2574,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>154</v>
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
@@ -2273,7 +2601,7 @@
         <v>99</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
         <v>110</v>
@@ -2364,117 +2692,117 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D16" s="23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="23"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="21" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="16"/>
+      <c r="A23" s="22"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" t="s">
         <v>151</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s">
         <v>152</v>
-      </c>
-      <c r="C26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D26" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2513,12 +2841,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{222693BF-2BFF-A046-AB6E-554C709C3F5D}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2530,12 +2858,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2544,34 +2872,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -2588,24 +2916,24 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="27"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
@@ -2615,10 +2943,10 @@
         <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2860,9 +3188,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>150</v>
-      </c>
+      <c r="A27" s="7"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="2"/>
@@ -2883,12 +3209,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4944CD94-FD2E-8C46-9AAC-EAC0C9A6262F}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2900,12 +3226,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2914,34 +3240,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -2958,51 +3284,51 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>184</v>
+      <c r="B7" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3010,7 +3336,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3024,7 +3350,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -3038,7 +3364,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3052,7 +3378,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3066,7 +3392,7 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3076,110 +3402,110 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D18" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>180</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="18" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="22"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="25"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -3203,25 +3529,25 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D319A960-7508-DA4B-86DA-8E2A767D7247}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -3234,12 +3560,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3248,34 +3574,34 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="14"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="C3" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="16"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -3292,51 +3618,51 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>154</v>
+      <c r="C7" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
         <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3344,7 +3670,7 @@
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -3358,7 +3684,7 @@
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -3372,7 +3698,7 @@
         <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -3386,7 +3712,7 @@
         <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
@@ -3400,7 +3726,7 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -3410,117 +3736,117 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="22"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="23"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>200</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C18" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="D18" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="22"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="23"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="23"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="21" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="21"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="18" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="22"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C22" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="16"/>
-    </row>
-    <row r="24" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="18" t="s">
+      <c r="C24" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="22"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="19"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="25" t="s">
-        <v>206</v>
-      </c>
-      <c r="B26" s="26" t="s">
-        <v>205</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>158</v>
-      </c>
-      <c r="D26" s="26" t="s">
-        <v>153</v>
+      <c r="C26" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3545,15 +3871,15 @@
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:D5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>